<commit_message>
New thing with undistort image
</commit_message>
<xml_diff>
--- a/laplai.xlsx
+++ b/laplai.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\setup files\NVIDIA\darkflow-master\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,13 +15,13 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +58,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -99,7 +112,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -131,9 +144,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,6 +179,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -340,24 +355,483 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-1.0661202214239369</v>
+      </c>
+      <c r="B2">
+        <v>41.044692554152768</v>
+      </c>
+      <c r="E2">
+        <v>-25.09</v>
+      </c>
+      <c r="F2">
+        <v>24.64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-26.975891345098439</v>
+      </c>
+      <c r="B3">
+        <v>24.26290552166828</v>
+      </c>
+      <c r="E3">
+        <v>-24.98</v>
+      </c>
+      <c r="F3">
+        <v>24.99</v>
+      </c>
+      <c r="H3">
+        <f>ABS(A4-$A$3)</f>
+        <v>0.14551096740033032</v>
+      </c>
+      <c r="I3">
+        <f>ABS(B4-$B$3)</f>
+        <v>0.52552188595111105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-26.830380377698109</v>
+      </c>
+      <c r="B4">
+        <v>24.788427407619391</v>
+      </c>
+      <c r="E4">
+        <v>-25.03</v>
+      </c>
+      <c r="F4">
+        <v>24.82</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H21" si="0">ABS(A5-$A$3)</f>
+        <v>4.8215443615760023E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I22" si="1">ABS(B5-$B$3)</f>
+        <v>0.13310514954865837</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-26.927675901482679</v>
+      </c>
+      <c r="B5">
+        <v>24.396010671216938</v>
+      </c>
+      <c r="E5">
+        <v>-25.05</v>
+      </c>
+      <c r="F5">
+        <v>24.74</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.7420815578452107E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.13741881737261963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-27.003312160676892</v>
+      </c>
+      <c r="B6">
+        <v>24.12548670429566</v>
+      </c>
+      <c r="E6">
+        <v>-25</v>
+      </c>
+      <c r="F6">
+        <v>24.91</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.244307037499226E-3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2.3362062256850891E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-26.977135652135939</v>
+      </c>
+      <c r="B7">
+        <v>24.286267583925131</v>
+      </c>
+      <c r="E7">
+        <v>-25.03</v>
+      </c>
+      <c r="F7">
+        <v>24.88</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.31909750524459923</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.73678382011858901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-26.65679383985384</v>
+      </c>
+      <c r="B8">
+        <v>24.999689341786869</v>
+      </c>
+      <c r="E8">
+        <v>-25.05</v>
+      </c>
+      <c r="F8">
+        <v>24.74</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.30905246847629897</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.6773776179783404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-26.66683887662214</v>
+      </c>
+      <c r="B9">
+        <v>24.94028313964662</v>
+      </c>
+      <c r="E9">
+        <v>-25.03</v>
+      </c>
+      <c r="F9">
+        <v>24.82</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.31880942611942942</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.82437504809038131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-26.65708191897901</v>
+      </c>
+      <c r="B10">
+        <v>25.087280569758661</v>
+      </c>
+      <c r="E10">
+        <v>-25.09</v>
+      </c>
+      <c r="F10">
+        <v>24.64</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.26405215765124979</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.69375252555940037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-26.71183918744719</v>
+      </c>
+      <c r="B11">
+        <v>24.95665804722768</v>
+      </c>
+      <c r="E11">
+        <v>-25.06</v>
+      </c>
+      <c r="F11">
+        <v>24.73</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.15840008394019023</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.53328843224278089</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-26.817491261158249</v>
+      </c>
+      <c r="B12">
+        <v>24.796193953911061</v>
+      </c>
+      <c r="E12">
+        <v>-25.03</v>
+      </c>
+      <c r="F12">
+        <v>24.82</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.1378103833067712</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0.45045543505186103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-26.838080961791668</v>
+      </c>
+      <c r="B13">
+        <v>24.713360956720141</v>
+      </c>
+      <c r="E13">
+        <v>-25.11</v>
+      </c>
+      <c r="F13">
+        <v>24.56</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.10468386519092832</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.37043870086870001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-26.871207479907511</v>
+      </c>
+      <c r="B14">
+        <v>24.63334422253698</v>
+      </c>
+      <c r="E14">
+        <v>-25</v>
+      </c>
+      <c r="F14">
+        <v>24.91</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.15838103613840815</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.57729082995210845</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-26.817510308960031</v>
+      </c>
+      <c r="B15">
+        <v>24.840196351620389</v>
+      </c>
+      <c r="E15">
+        <v>-25.1</v>
+      </c>
+      <c r="F15">
+        <v>24.75</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>8.1122523128779989E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.35469270544930964</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-26.894768821969659</v>
+      </c>
+      <c r="B16">
+        <v>24.61759822711759</v>
+      </c>
+      <c r="E16">
+        <v>-25</v>
+      </c>
+      <c r="F16">
+        <v>24.9</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.31702372581372984</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0.75151461935831065</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-26.65886761928471</v>
+      </c>
+      <c r="B17">
+        <v>25.014420141026591</v>
+      </c>
+      <c r="E17">
+        <v>-25</v>
+      </c>
+      <c r="F17">
+        <v>24.97</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.3657875095687082</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0.72905467425427162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-26.610103835529731</v>
+      </c>
+      <c r="B18">
+        <v>24.991960195922552</v>
+      </c>
+      <c r="E18">
+        <v>-24.95</v>
+      </c>
+      <c r="F18">
+        <v>25.02</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.33267166924811065</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.74438630061235855</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-26.643219675850329</v>
+      </c>
+      <c r="B19">
+        <v>25.007291822280639</v>
+      </c>
+      <c r="E19">
+        <v>-25.08</v>
+      </c>
+      <c r="F19">
+        <v>24.53</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.15261202647662842</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0.13893140079535016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-26.823279318621811</v>
+      </c>
+      <c r="B20">
+        <v>24.40183692246363</v>
+      </c>
+      <c r="E20">
+        <v>-24.95</v>
+      </c>
+      <c r="F20">
+        <v>25.08</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.20621938724827871</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.60605628144681845</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-26.769671957850161</v>
+      </c>
+      <c r="B21">
+        <v>24.868961803115099</v>
+      </c>
+      <c r="E21">
+        <v>-24.97</v>
+      </c>
+      <c r="F21">
+        <v>25.06</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.23051595588436058</v>
+      </c>
+      <c r="I21">
+        <f>ABS(B22-$B$3)</f>
+        <v>0.64616156434487948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-26.745375389214079</v>
+      </c>
+      <c r="B22">
+        <v>24.90906708601316</v>
+      </c>
+      <c r="H22">
+        <f>AVERAGE(H3:H21)</f>
+        <v>0.19361217142465859</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(I3:I21)</f>
+        <v>0.50810357217119473</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>